<commit_message>
new custom properties shorter and some optional
</commit_message>
<xml_diff>
--- a/sample lightweight domain/resources/domains/currencies.xlsx
+++ b/sample lightweight domain/resources/domains/currencies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FREDERICMercier\Desktop\VALUE PROVIDER\1- mine\workspace\sample2-bom2\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IBM\GitHub\dc-lightweight-domain\sample lightweight domain\resources\domains\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD8CE2A-ADE8-4A2D-8C14-ADAE21CF0AC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC2097B-A7BD-4D54-B097-119DE5127BFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{191EE4D9-30B1-4391-94EB-FEF0069EDE9A}"/>
+    <workbookView xWindow="5070" yWindow="285" windowWidth="17625" windowHeight="15345" xr2:uid="{191EE4D9-30B1-4391-94EB-FEF0069EDE9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Label</t>
-  </si>
-  <si>
-    <t>Values</t>
   </si>
   <si>
     <t>BOM to XOM</t>
@@ -412,104 +409,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746568ED-BE32-48AD-BB23-CCB4654E692A}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>SUBSTITUTE(C2, " ", "_")</f>
-        <v>US_Dollar</v>
-      </c>
       <c r="B2" t="str">
-        <f>CONCATENATE("return """, UPPER(LEFT(A2,4)), """;")</f>
-        <v>return "US_D";</v>
-      </c>
-      <c r="C2" t="s">
+        <f>CONCATENATE("return """, SUBSTITUTE(UPPER(LEFT(A2,4)), " ", ""), """;")</f>
+        <v>return "USD";</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A64" si="0">SUBSTITUTE(C3, " ", "_")</f>
-        <v>Euro</v>
-      </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B62" si="1">CONCATENATE("return """, UPPER(LEFT(A3,4)), """;")</f>
+        <f t="shared" ref="B3:B7" si="0">CONCATENATE("return """, SUBSTITUTE(UPPER(LEFT(A3,4)), " ", ""), """;")</f>
         <v>return "EURO";</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
+      <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>Pound</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="1"/>
         <v>return "POUN";</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
+      <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>JP_Yen</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="1"/>
-        <v>return "JP_Y";</v>
-      </c>
-      <c r="C5" t="s">
+        <v>return "JPY";</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
+      <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>PRC_RMB</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="1"/>
-        <v>return "PRC_";</v>
-      </c>
-      <c r="C6" t="s">
+        <v>return "PRC";</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>SG_Dollar</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="1"/>
-        <v>return "SG_D";</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
+        <v>return "SGD";</v>
       </c>
     </row>
   </sheetData>

</xml_diff>